<commit_message>
screenshot folder creations updated with timestamp and screenshot path reading from teh excel to check and update accordingly
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ExcelData.xlsx
+++ b/src/test/resources/testData/ExcelData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28609"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3447089E-A96A-4B73-AD7B-C141D1E30332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{728B82FC-3DDC-4EC2-A339-615A2F08AC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
   <si>
     <t>testCaseId</t>
   </si>
@@ -101,12 +101,22 @@
   </si>
   <si>
     <t>zz</t>
+  </si>
+  <si>
+    <t>2025-02-20</t>
+  </si>
+  <si>
+    <t>Scenario1-20_02_2025_07_57_58</t>
+  </si>
+  <si>
+    <t>Scenario2-20_02_2025_07_58_36</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -489,18 +499,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -628,16 +638,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB505FAB-046B-4F84-A640-A57AFC158940}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -673,83 +683,128 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>10</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>11</v>
       </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="E4"/>
+      <c r="F4"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>12</v>
       </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
+      <c r="E5"/>
+      <c r="F5"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>14</v>
       </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
+      <c r="E6"/>
+      <c r="F6"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>16</v>
       </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
+      <c r="E7"/>
+      <c r="F7"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>18</v>
       </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
+      <c r="E8"/>
+      <c r="F8"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>20</v>
       </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
+      <c r="E9"/>
+      <c r="F9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>